<commit_message>
Fixed navigation issues, added timer UI, NEED TO SEPARATE GeneralController into TimerController. Need to figure out how to run 2 controllers on 1 fxml. Need to make menu disabled while timer is running.
</commit_message>
<xml_diff>
--- a/CAB302 Database.xlsx
+++ b/CAB302 Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\OneDrive\Documents\Uni\Y3 S1\CAB302\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyAnd\IdeaProjects\Group-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFEB79C-5C29-4669-8BCB-1E50FAD3227C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013F4461-8F51-46D2-AF88-CFDC1A20E7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCA21922-E96C-4113-889B-95ADB48960DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{CCA21922-E96C-4113-889B-95ADB48960DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t>User Credentials</t>
   </si>
@@ -294,19 +294,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -644,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B61B567-27DB-465F-8E23-E3562BCB3DEA}">
   <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,10 +721,10 @@
       <c r="E5">
         <v>1234567890</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>43</v>
       </c>
       <c r="I5" t="s">
@@ -739,10 +736,10 @@
       <c r="K5" s="2">
         <v>0.16666666666666666</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="6" t="s">
         <v>60</v>
       </c>
       <c r="N5" t="s">
@@ -762,10 +759,10 @@
       <c r="E6">
         <v>2345678901</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I6" t="s">
@@ -777,10 +774,10 @@
       <c r="K6" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="6" t="s">
         <v>62</v>
       </c>
       <c r="N6" t="s">
@@ -800,10 +797,10 @@
       <c r="E7">
         <v>3456789012</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>45</v>
       </c>
       <c r="I7" t="s">
@@ -815,10 +812,10 @@
       <c r="K7" s="2">
         <v>0.125</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="6" t="s">
         <v>63</v>
       </c>
       <c r="N7" t="s">
@@ -838,10 +835,10 @@
       <c r="E8">
         <v>4567890123</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>46</v>
       </c>
       <c r="I8" t="s">
@@ -853,10 +850,10 @@
       <c r="K8" s="2">
         <v>0.125</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="L8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" s="6" t="s">
         <v>64</v>
       </c>
       <c r="N8" t="s">
@@ -876,27 +873,24 @@
       <c r="E9">
         <v>5678901234</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="L9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="L10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="L11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="8" t="s">
         <v>54</v>
       </c>
       <c r="I12" s="3" t="s">
@@ -908,7 +902,7 @@
       <c r="K12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="L12" s="3" t="s">
         <v>52</v>
       </c>
       <c r="M12" s="3"/>
@@ -917,10 +911,10 @@
       <c r="B13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I13" t="s">
@@ -932,7 +926,7 @@
       <c r="K13" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="L13" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -940,10 +934,10 @@
       <c r="F14" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>45</v>
       </c>
       <c r="I14" t="s">
@@ -955,7 +949,7 @@
       <c r="K14" s="2">
         <v>0.125</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="L14" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -975,13 +969,13 @@
       <c r="F15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" t="s">
         <v>50</v>
       </c>
       <c r="J15" s="1" t="s">
@@ -990,7 +984,7 @@
       <c r="K15" s="2">
         <v>0.125</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="6" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1012,7 +1006,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>2</v>
       </c>
@@ -1030,7 +1024,7 @@
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>3</v>
       </c>
@@ -1047,7 +1041,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>4</v>
       </c>
@@ -1064,7 +1058,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>5</v>
       </c>
@@ -1081,9 +1075,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>38</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1107,15 +1107,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B2D02817A78AA478C8708738F271F07" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfbaadc1ccab3b73a3825334463bf26e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a427e027-16f2-4b60-acb3-29aa6bca2897" xmlns:ns4="3f493cb4-3cec-4ed5-b80c-3b936ab9c96e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="494b1dbebb6c483d0f616a3faad70084" ns3:_="" ns4:_="">
     <xsd:import namespace="a427e027-16f2-4b60-acb3-29aa6bca2897"/>
@@ -1344,6 +1335,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1353,14 +1353,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5234D896-0EFD-44FF-ABF9-7C9B0E64FE60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2836C2FE-3B52-44E0-BB62-AF6947216FC8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1375,6 +1367,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5234D896-0EFD-44FF-ABF9-7C9B0E64FE60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>